<commit_message>
Task 7 at Project_Playground
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/PM-SHEET.xlsx
+++ b/01_ProjectPlanning/PM-SHEET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Documents\Schule\SYP\Trimbacher-Tumfart_Project_SYP\01_ProjectPlanning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Schule\Syp\Trimbacher-Tumfart_Project_SYP\01_ProjectPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D9C12D3-230A-453C-97DD-9C9AD426B559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80088D95-24D7-4E38-B2E7-19DBB9524BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95D66045-7A69-48E7-A637-FD7DD8CC0083}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{95D66045-7A69-48E7-A637-FD7DD8CC0083}"/>
   </bookViews>
   <sheets>
     <sheet name="PM-SHEET" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>TASK</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>storing data in local fiels</t>
+  </si>
+  <si>
+    <t>Tumfart/Trimbacher</t>
+  </si>
+  <si>
+    <t>Informing abou Android Std.</t>
   </si>
 </sst>
 </file>
@@ -447,21 +453,21 @@
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -500,7 +506,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
@@ -514,12 +520,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" ref="F4:F5" si="0">D4-E4</f>
+        <f t="shared" ref="F4" si="0">D4-E4</f>
         <v>3</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -538,7 +544,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -557,15 +563,28 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2">
+        <f>D7-E7</f>
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>

</xml_diff>